<commit_message>
Version 0.5 for load data for original plan
</commit_message>
<xml_diff>
--- a/excel/BomPlan.xlsx
+++ b/excel/BomPlan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>Quantity</t>
   </si>
@@ -40,15 +40,37 @@
   </si>
   <si>
     <t>SAID</t>
+  </si>
+  <si>
+    <t>TB</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>TS</t>
+  </si>
+  <si>
+    <t>BS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -90,9 +112,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="12" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="12" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="12" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F7"/>
+  <dimension ref="B2:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,7 +442,7 @@
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
@@ -421,38 +458,55 @@
       <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="1">
         <v>50</v>
       </c>
-      <c r="D3" s="1">
-        <v>84.625</v>
-      </c>
-      <c r="E3" s="1">
-        <v>45.625</v>
+      <c r="D3" s="3">
+        <v>88.25</v>
+      </c>
+      <c r="E3" s="8">
+        <v>46.875</v>
       </c>
       <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="1"/>
+      <c r="H3" s="1">
+        <v>300</v>
+      </c>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="1">
         <v>40</v>
       </c>
-      <c r="D4" s="1">
-        <v>69.125</v>
-      </c>
-      <c r="E4" s="1">
-        <v>30.125</v>
+      <c r="D4" s="4">
+        <v>116.125</v>
+      </c>
+      <c r="E4" s="8">
+        <v>45.625</v>
       </c>
       <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="1"/>
+      <c r="H4" s="1">
+        <v>400</v>
+      </c>
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
@@ -461,11 +515,16 @@
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="1">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="5">
+        <v>11</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1">
+        <v>400</v>
+      </c>
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -474,11 +533,16 @@
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="1">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F6" s="5">
+        <v>17</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1">
+        <v>500</v>
+      </c>
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
@@ -487,9 +551,56 @@
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="1">
-        <v>12.5</v>
-      </c>
+      <c r="F7" s="5">
+        <v>3</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="1">
+        <v>300</v>
+      </c>
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="2">
+        <v>40</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="5">
+        <v>17</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="2">
+        <v>500</v>
+      </c>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="6"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="6"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
1. New import file and parameters
2. Data valid check for each table
</commit_message>
<xml_diff>
--- a/excel/BomPlan.xlsx
+++ b/excel/BomPlan.xlsx
@@ -431,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I10"/>
+  <dimension ref="B2:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,7 +442,7 @@
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
@@ -466,7 +466,7 @@
       </c>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -476,7 +476,7 @@
       <c r="D3" s="3">
         <v>88.25</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3">
         <v>46.875</v>
       </c>
       <c r="F3" s="1"/>
@@ -485,8 +485,11 @@
         <v>300</v>
       </c>
       <c r="I3" s="6"/>
-    </row>
-    <row r="4" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <v>46.875</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
@@ -506,7 +509,7 @@
       </c>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
@@ -524,7 +527,7 @@
       </c>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -542,7 +545,7 @@
       </c>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
@@ -552,7 +555,7 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>10</v>
@@ -562,7 +565,7 @@
       </c>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
@@ -582,7 +585,7 @@
       </c>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="6"/>
       <c r="C9" s="7"/>
       <c r="D9" s="6"/>
@@ -592,7 +595,7 @@
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="C10" s="7"/>
       <c r="D10" s="6"/>

</xml_diff>

<commit_message>
Import and calculate completely
</commit_message>
<xml_diff>
--- a/excel/BomPlan.xlsx
+++ b/excel/BomPlan.xlsx
@@ -434,7 +434,7 @@
   <dimension ref="B2:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E4" sqref="D3:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,7 +555,7 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="5">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
some modification for SEDPlan
1. the head reports are modified
2. multiple Fabrication Lists can be selected to generate the SubAssembly List
3. Add project no into system, cs code is modified, but sql scripts not yet.
</commit_message>
<xml_diff>
--- a/excel/BomPlan.xlsx
+++ b/excel/BomPlan.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BOMPlanTest" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="FAB01-B3-02" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="15">
   <si>
     <t>Quantity</t>
   </si>
@@ -52,6 +52,15 @@
   </si>
   <si>
     <t>BS</t>
+  </si>
+  <si>
+    <t>Project No:</t>
+  </si>
+  <si>
+    <t>S32A1305700</t>
+  </si>
+  <si>
+    <t>Color Code</t>
   </si>
 </sst>
 </file>
@@ -431,171 +440,173 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="D3:E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="6"/>
-    </row>
-    <row r="3" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1">
-        <v>50</v>
-      </c>
-      <c r="D3" s="3">
-        <v>88.25</v>
-      </c>
-      <c r="E3">
-        <v>46.875</v>
-      </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1">
-        <v>300</v>
-      </c>
-      <c r="I3" s="6"/>
-      <c r="L3">
-        <v>46.875</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I3" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="1">
-        <v>40</v>
-      </c>
-      <c r="D4" s="4">
-        <v>116.125</v>
-      </c>
-      <c r="E4" s="8">
-        <v>45.625</v>
+        <v>50</v>
+      </c>
+      <c r="D4" s="3">
+        <v>88.25</v>
+      </c>
+      <c r="E4">
+        <v>46.875</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1">
-        <v>400</v>
-      </c>
-      <c r="I4" s="6"/>
-    </row>
-    <row r="5" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+        <v>300</v>
+      </c>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1">
-        <v>10</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="5">
-        <v>11</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="D5" s="4">
+        <v>116.125</v>
+      </c>
+      <c r="E5" s="8">
+        <v>45.625</v>
+      </c>
+      <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1">
         <v>400</v>
       </c>
-      <c r="I5" s="6"/>
-    </row>
-    <row r="6" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="1">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="5">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1">
-        <v>500</v>
-      </c>
-      <c r="I6" s="6"/>
-    </row>
-    <row r="7" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+        <v>400</v>
+      </c>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="5">
-        <v>3</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>10</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="G7" s="1"/>
       <c r="H7" s="1">
-        <v>300</v>
-      </c>
-      <c r="I7" s="6"/>
-    </row>
-    <row r="8" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="2">
-        <v>40</v>
+      <c r="C8" s="1">
+        <v>30</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="5">
+        <v>3</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="1">
+        <v>300</v>
+      </c>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="2">
+        <v>40</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="5">
         <v>17</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H9" s="2">
         <v>500</v>
       </c>
-      <c r="I8" s="6"/>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="6"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="C10" s="7"/>
       <c r="D10" s="6"/>
@@ -612,12 +623,170 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3">
+        <v>88.25</v>
+      </c>
+      <c r="E4">
+        <v>46.875</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1">
+        <v>300</v>
+      </c>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>11</v>
+      </c>
+      <c r="D5" s="4">
+        <v>116.125</v>
+      </c>
+      <c r="E5" s="8">
+        <v>45.625</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1">
+        <v>400</v>
+      </c>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="5">
+        <v>11</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1">
+        <v>400</v>
+      </c>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="5">
+        <v>17</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1">
+        <v>500</v>
+      </c>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1">
+        <v>14</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="5">
+        <v>3</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="1">
+        <v>300</v>
+      </c>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1">
+        <v>15</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="5">
+        <v>17</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="2">
+        <v>500</v>
+      </c>
+      <c r="I9" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Complete C# coding, SQL scripts and test for following 3 new functions
1. Project No and Name complete
2. Description for SA complete.
3. Color of SA in BOM Plan and of Detail Design in Fixed weight complete.
</commit_message>
<xml_diff>
--- a/excel/BomPlan.xlsx
+++ b/excel/BomPlan.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -11,12 +11,12 @@
     <sheet name="FAB01-B3-02" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
   <si>
     <t>Quantity</t>
   </si>
@@ -61,28 +61,91 @@
   </si>
   <si>
     <t>Color Code</t>
+  </si>
+  <si>
+    <t>TS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RAL5011</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RAL5013</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RAL5013</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RAL5012</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RAL5010</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SA-Test1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SA-Test2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SA-Test3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Color Code</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>S32A1305700</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RBL5010</t>
+  </si>
+  <si>
+    <t>RBL5011</t>
+  </si>
+  <si>
+    <t>RBL5012</t>
+  </si>
+  <si>
+    <t>RBL5013</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="176" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -131,7 +194,7 @@
     <xf numFmtId="12" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -141,7 +204,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -154,7 +217,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -228,7 +291,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -263,7 +325,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -439,21 +500,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -461,10 +522,10 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
@@ -490,7 +551,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="14.25">
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
@@ -508,9 +569,11 @@
       <c r="H4" s="1">
         <v>300</v>
       </c>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="14.25">
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
@@ -528,9 +591,11 @@
       <c r="H5" s="1">
         <v>400</v>
       </c>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="14.25">
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -546,9 +611,11 @@
       <c r="H6" s="1">
         <v>400</v>
       </c>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I6" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="14.25">
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
@@ -564,9 +631,11 @@
       <c r="H7" s="1">
         <v>500</v>
       </c>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="14.25">
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
@@ -584,9 +653,11 @@
       <c r="H8" s="1">
         <v>300</v>
       </c>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I8" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="14.25">
       <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
@@ -604,9 +675,11 @@
       <c r="H9" s="2">
         <v>500</v>
       </c>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I9" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="B10" s="6"/>
       <c r="C10" s="7"/>
       <c r="D10" s="6"/>
@@ -617,34 +690,35 @@
       <c r="I10" s="6"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="I4" sqref="I4:I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
@@ -667,12 +741,12 @@
         <v>9</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="14.25">
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1">
         <v>10</v>
@@ -688,11 +762,13 @@
       <c r="H4" s="1">
         <v>300</v>
       </c>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I4" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="14.25">
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C5" s="1">
         <v>11</v>
@@ -708,11 +784,13 @@
       <c r="H5" s="1">
         <v>400</v>
       </c>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I5" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="14.25">
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C6" s="1">
         <v>12</v>
@@ -726,9 +804,11 @@
       <c r="H6" s="1">
         <v>400</v>
       </c>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I6" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="14.25">
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
@@ -744,11 +824,13 @@
       <c r="H7" s="1">
         <v>500</v>
       </c>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I7" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="14.25">
       <c r="B8" s="1" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C8" s="1">
         <v>14</v>
@@ -759,14 +841,16 @@
         <v>3</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H8" s="1">
         <v>300</v>
       </c>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I8" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="14.25">
       <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
@@ -784,21 +868,26 @@
       <c r="H9" s="2">
         <v>500</v>
       </c>
-      <c r="I9" s="1"/>
+      <c r="I9" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
some modification on report template
</commit_message>
<xml_diff>
--- a/excel/BomPlan.xlsx
+++ b/excel/BomPlan.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SAB01-B2-00" sheetId="1" r:id="rId1"/>
     <sheet name="SAB01-B2-01" sheetId="4" r:id="rId2"/>
-    <sheet name="SAB01-B3-02" sheetId="2" r:id="rId3"/>
+    <sheet name="SAB-BCV01-B03 02" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -125,26 +125,26 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -195,7 +195,7 @@
     <xf numFmtId="12" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -205,7 +205,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -218,7 +218,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -510,14 +510,14 @@
       <selection sqref="A1:I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -525,10 +525,10 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9">
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9">
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
@@ -554,7 +554,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" ht="15.75">
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
@@ -576,7 +576,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" ht="15.75">
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
@@ -598,7 +598,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" ht="15.75">
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -618,7 +618,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" ht="15.75">
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
@@ -638,7 +638,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" ht="15.75">
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
@@ -660,7 +660,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" ht="15.75">
       <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
@@ -682,7 +682,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9">
       <c r="B10" s="6"/>
       <c r="C10" s="7"/>
       <c r="D10" s="6"/>
@@ -702,13 +702,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -716,10 +716,10 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9">
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9">
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
@@ -745,7 +745,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" ht="15.75">
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
@@ -767,7 +767,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" ht="15.75">
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
@@ -789,7 +789,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" ht="15.75">
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -809,7 +809,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" ht="15.75">
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
@@ -829,7 +829,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" ht="15.75">
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
@@ -851,7 +851,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" ht="15.75">
       <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
@@ -884,18 +884,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -903,7 +903,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9">
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
@@ -929,7 +929,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" ht="15.75">
       <c r="B4" s="1" t="s">
         <v>21</v>
       </c>
@@ -951,7 +951,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" ht="15.75">
       <c r="B5" s="1" t="s">
         <v>21</v>
       </c>
@@ -973,7 +973,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" ht="15.75">
       <c r="B6" s="1" t="s">
         <v>22</v>
       </c>
@@ -993,7 +993,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" ht="15.75">
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1013,7 +1013,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" ht="15.75">
       <c r="B8" s="1" t="s">
         <v>23</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" ht="15.75">
       <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
@@ -1070,7 +1070,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
1. Added Sub SA calculation. Because some SA's has sub SA components which have separate part lists, so sub SA should be calculated into BOM fabrication list;
	1) added a field in SA_Component to mark if it is a sub SA;
	2) Modified some checking function to accept sub SA;
	3) Moved checking function into "insert" stored procedure and show checking errors to users
	4) Modified stp_CalBomPlan to calculate sub SA into result

2. Added a parameter for BOM Plan that indicates the motor position of some SA.

	1) Added DBO.FUN_CALBP_LRNUM to get the quantity of LHS or RHS according to motor position of SA

3. Modified ExcelDataImport.cs to accept the column name in Excel without units.
</commit_message>
<xml_diff>
--- a/excel/BomPlan.xlsx
+++ b/excel/BomPlan.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="33">
   <si>
     <t>Quantity</t>
   </si>
@@ -118,6 +118,15 @@
   </si>
   <si>
     <t>RBL5013</t>
+  </si>
+  <si>
+    <t>EW</t>
+  </si>
+  <si>
+    <t>LR</t>
+  </si>
+  <si>
+    <t>R</t>
   </si>
 </sst>
 </file>
@@ -882,20 +891,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -903,7 +912,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:11">
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
@@ -926,10 +935,16 @@
         <v>9</v>
       </c>
       <c r="I3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75">
+    <row r="4" spans="1:11" ht="15.75">
       <c r="B4" s="1" t="s">
         <v>21</v>
       </c>
@@ -947,11 +962,15 @@
       <c r="H4" s="1">
         <v>300</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="1"/>
+      <c r="J4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75">
+    <row r="5" spans="1:11" ht="15.75">
       <c r="B5" s="1" t="s">
         <v>21</v>
       </c>
@@ -969,11 +988,17 @@
       <c r="H5" s="1">
         <v>400</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="1">
+        <v>1000</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75">
+    <row r="6" spans="1:11" ht="15.75">
       <c r="B6" s="1" t="s">
         <v>22</v>
       </c>
@@ -989,11 +1014,15 @@
       <c r="H6" s="1">
         <v>400</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="1"/>
+      <c r="J6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75">
+    <row r="7" spans="1:11" ht="15.75">
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1009,11 +1038,15 @@
       <c r="H7" s="1">
         <v>500</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="1"/>
+      <c r="J7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75">
+    <row r="8" spans="1:11" ht="15.75">
       <c r="B8" s="1" t="s">
         <v>23</v>
       </c>
@@ -1031,11 +1064,17 @@
       <c r="H8" s="1">
         <v>300</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="1">
+        <v>1500</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.75">
+    <row r="9" spans="1:11" ht="15.75">
       <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
@@ -1053,7 +1092,11 @@
       <c r="H9" s="2">
         <v>500</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" s="2"/>
+      <c r="J9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K9" s="1" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>